<commit_message>
Schedule update: talk titles
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\wahl\.Transfers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\wahl\.Repositories\EAE-Memorial-Symposium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D271A909-F705-4083-8E92-960D4A8628AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8198537-96D6-464D-9C87-DFE78D1822A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{6CF8EB66-4F5C-458A-9E7A-DF70772FA9B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Time</t>
   </si>
@@ -115,6 +115,24 @@
       <t xml:space="preserve"> Break —</t>
     </r>
   </si>
+  <si>
+    <t>Presentation Title</t>
+  </si>
+  <si>
+    <t>Allen Emerson: A Mind for Theory</t>
+  </si>
+  <si>
+    <t>Allen Emerson and Me: A Personal History</t>
+  </si>
+  <si>
+    <t>(TBD)</t>
+  </si>
+  <si>
+    <t>Kedar Namjoshi, Thomas Wahl</t>
+  </si>
+  <si>
+    <t>Allen Emerson's Contributions to the Automata-Theoretic Approach</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +203,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -223,19 +248,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color indexed="64"/>
       </left>
@@ -301,19 +313,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,56 +412,92 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,196 +836,240 @@
   <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="44.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
+      <c r="D2" s="31" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>0.375</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>0.38194444444444442</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="D5" s="26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>0.40972222222222221</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>0.4236111111111111</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <v>0.4375</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="21" t="s">
         <v>6</v>
       </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="24" t="s">
         <v>17</v>
       </c>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>0.5</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="28"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="20" t="s">
         <v>8</v>
       </c>
+      <c r="D13" s="29" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>0.59722222222222221</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="20" t="s">
         <v>9</v>
       </c>
+      <c r="D14" s="26" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <v>0.61111111111111116</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="24" t="s">
         <v>10</v>
       </c>
+      <c r="D15" s="30"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="17" t="s">
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="9">
+      <c r="C17" s="25"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="6">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="9">
+      <c r="D18" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="6">
         <v>0.68055555555555558</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="9">
+      <c r="D19" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="6">
         <v>0.69444444444444442</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="9">
+      <c r="D20" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="6">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="9">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="6">
         <v>0.72222222222222221</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="13">
+    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="8">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding open mike for session 2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\wahl\.Repositories\EAE-Memorial-Symposium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kedar/github/CAV-Allen-Symposium/EAE-Memorial-Symposium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E926BB7-AE08-4D85-B45D-25C54122B095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012E709-C70B-3B40-86C3-EC5DC43A69C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{6CF8EB66-4F5C-458A-9E7A-DF70772FA9B8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{6CF8EB66-4F5C-458A-9E7A-DF70772FA9B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Time</t>
   </si>
@@ -830,21 +830,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B582FB-959F-449C-8FAB-D7436FE6FE6F}">
-  <dimension ref="B1:H24"/>
+  <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -855,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6">
         <v>0.375</v>
       </c>
@@ -866,7 +866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="6">
         <v>0.38194444444444442</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -884,7 +884,7 @@
       </c>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>0.40972222222222221</v>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <v>0.4236111111111111</v>
       </c>
@@ -902,7 +902,7 @@
       </c>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>0.4375</v>
       </c>
@@ -911,14 +911,14 @@
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="28"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <v>0.45833333333333331</v>
       </c>
@@ -927,134 +927,143 @@
       </c>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
         <v>0.5</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="29" t="s">
+      <c r="D12" s="19"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="6">
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D14" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="6">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="6">
         <v>0.59722222222222221</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="6">
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="6">
         <v>0.61111111111111116</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="6">
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="6">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="32" t="s">
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="6">
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="6">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="6">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="6">
         <v>0.68055555555555558</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="6">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="6">
         <v>0.69444444444444442</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C21" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="6">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="6">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="6">
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="6">
         <v>0.72222222222222221</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="8">
+    <row r="24" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="2:4" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>